<commit_message>
Update correlation.py and datapoints.xlsx
</commit_message>
<xml_diff>
--- a/data/datapoints.xlsx
+++ b/data/datapoints.xlsx
@@ -1,52 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobif\OneDrive\Desktop\Coding\Code-Complexity-Research\complexity-verification-project\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EB72E14-8C40-48DC-9068-BA231865ECDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{992B0E78-ED9F-4646-B363-F95E7BE0922B}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="cog_dataset_1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="cog_dataset_3" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="fMRI_dataset" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -65,21 +48,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -379,12 +421,555 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96CCF4FD-B992-4780-AF10-97E05CA71075}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>3.74</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4.03</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.18</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2.18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3.62</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>4.13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>3.64</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>3.53</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3.03</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>3.74</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>3.26</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>3.73</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2.73</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2.09</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>3.27</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>4.02</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>4.35</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2.57</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>3.28</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>4.07</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>3.92</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>2.63</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>2.71</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>3.77</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>3.47</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>4.02</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>3.82</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>2.28</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>3.34</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>4.15</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>3.23</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>4.07</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>2.12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>